<commit_message>
added a few more
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -92,6 +92,45 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Searching for references to bolter / support the prediction that male and female IFD should be the same.
+- papers that cite Petkov 
+-citations within Payseur and Otto
+- citations within Shapley et al review
+- citations within WangR SC review
+- known oocyte cytology papers</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 Searching for references to bolter / support the prediction that female SC are longer than male
 *birds!
 -Borodin papers
@@ -103,8 +142,82 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Searching for references to bolter / support the prediction that female SC are longer than male
+*birds!
+-Borodin papers
+*Fish</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Searching for references to bolter / support the prediction that female SC are longer than male
+*birds!
+-Borodin papers
+*Fish</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -278,6 +391,18 @@
   </si>
   <si>
     <t>female less dense CO landscape</t>
+  </si>
+  <si>
+    <t>Wang (kleckner)</t>
+  </si>
+  <si>
+    <t>COI, CO maturation and humand aneuploidy</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>High-res sex-specific linkage maps of mouse reveal polarized distribution of CO in male germline</t>
   </si>
 </sst>
 </file>
@@ -631,10 +756,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,69 +831,88 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2019</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2014</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2016</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -775,78 +920,70 @@
         <v>2016</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>2018</v>
       </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2016</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2018</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2016</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>2019</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B22" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G18" r:id="rId1" location="Sec8" display="https://www.nature.com/articles/srep37698 - Sec8"/>
+    <hyperlink ref="G15" r:id="rId1" location="Sec8" display="https://www.nature.com/articles/srep37698 - Sec8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -855,21 +992,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -877,8 +1037,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -887,7 +1059,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,27 +1152,73 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add notes and papers to read for DMC1 background
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
-    <sheet name="CO Rec landscale" sheetId="3" r:id="rId2"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId3"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId4"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId5"/>
+    <sheet name="DSB.DMC1" sheetId="7" r:id="rId2"/>
+    <sheet name="CO Rec landscale" sheetId="3" r:id="rId3"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId4"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId5"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId6"/>
+    <sheet name="SC general" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -72,7 +74,7 @@
     <author>PETERSON, APRIL L</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,10 +133,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Searching for references to bolter / support the prediction that female SC are longer than male
-*birds!
--Borodin papers
-*Fish</t>
+Searching for references to bolter / support the prediction that male and female IFD should be the same.
+- papers that cite Petkov 
+-citations within Payseur and Otto
+- citations within Shapley et al review
+- citations within WangR SC review
+- known oocyte cytology papers</t>
         </r>
       </text>
     </comment>
@@ -216,8 +220,82 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Searching for references to bolter / support the prediction that female SC are longer than male
+*birds!
+-Borodin papers
+*Fish</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Searching for references to bolter / support the prediction that female SC are longer than male
+*birds!
+-Borodin papers
+*Fish</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>Year</t>
   </si>
@@ -247,9 +325,6 @@
   </si>
   <si>
     <t>2 levels of interferen in mouse meiotic recomb</t>
-  </si>
-  <si>
-    <t>(found 2 classes of COs</t>
   </si>
   <si>
     <t>Cytological IFD measures?</t>
@@ -403,6 +478,75 @@
   </si>
   <si>
     <t>High-res sex-specific linkage maps of mouse reveal polarized distribution of CO in male germline</t>
+  </si>
+  <si>
+    <t>Dietrich and Mulder</t>
+  </si>
+  <si>
+    <t>electron ligh micro of ovaries</t>
+  </si>
+  <si>
+    <t>tomato early nodules and late nodules both have interference</t>
+  </si>
+  <si>
+    <t>MSH4, in WT and Sycp1 -/-.  (found 2 classes of COs / two types of interference, based on differences between interference of MSH4 and MLH1). Used FISH for chrms 1,2,18,19; calculated gamma distribution from chrm specific intervals.</t>
+  </si>
+  <si>
+    <t>Bollshweiler</t>
+  </si>
+  <si>
+    <t>archteure of SYCP3 fibre</t>
+  </si>
+  <si>
+    <t>SC AE is built on top of chromatin stru. The underlying loop str might be maintained.</t>
+  </si>
+  <si>
+    <t>(the ovaries from DeBoer 2006). Plot of time lines of prophase between for ovaries</t>
+  </si>
+  <si>
+    <t>EM spreads of male and females</t>
+  </si>
+  <si>
+    <t>early percursor markers in males (female / ovary spreads -- oocytes were also treated with immunocytology stains)</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>DMC1</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3907295/</t>
+  </si>
+  <si>
+    <t>Baier</t>
+  </si>
+  <si>
+    <t>Variation in Genome-Wide Levels of Meiotic</t>
+  </si>
+  <si>
+    <t>low medium and high rec mouse strains -- rank order DMC1, RAD51 matches (all cells are from Z stage)</t>
+  </si>
+  <si>
+    <t>Moens</t>
+  </si>
+  <si>
+    <t>Gruhn</t>
+  </si>
+  <si>
+    <t>Broner</t>
+  </si>
+  <si>
+    <t>Balcova, Forejt</t>
+  </si>
+  <si>
+    <t>Hybrid Sterility Locus on Chromosome X</t>
+  </si>
+  <si>
+    <t>To determine the RAD51/DMC1 foci count, we scored zygotene spermatocytes (predominantly inmid-zygonema) with bright signal of SCP3 and RAD51/DMC1. RAD51 and DMC1 proteins,  were labeled with the same secondary antibody and counted together. Altogether 4–5 animals. per strain and 20 or more cells per mouse were evaluated for bothMLH1 and RAD51/DMC1.</t>
+  </si>
+  <si>
+    <t>? CO homeostasis</t>
   </si>
 </sst>
 </file>
@@ -447,12 +591,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -468,13 +618,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -756,16 +908,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -783,13 +936,13 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -803,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -814,105 +967,115 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>2006</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>1983</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2019</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2014</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
+      <c r="C7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -920,70 +1083,89 @@
         <v>2016</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>2018</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2016</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2019</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>2018</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2016</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2019</v>
+      </c>
+      <c r="B26" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2016</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2019</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1" location="Sec8" display="https://www.nature.com/articles/srep37698 - Sec8"/>
+    <hyperlink ref="G18" r:id="rId1" location="Sec8" display="https://www.nature.com/articles/srep37698 - Sec8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -992,6 +1174,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2016</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1015,26 +1308,26 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,10 +1335,10 @@
         <v>2014</v>
       </c>
       <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1054,12 +1347,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,10 +1371,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,10 +1382,10 @@
         <v>2002</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,12 +1393,12 @@
         <v>2015</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,12 +1408,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,21 +1421,21 @@
         <v>2016</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1175,10 +1468,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1211,10 +1504,57 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notes of references, stuggle with bib
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
   <si>
     <t>Year</t>
   </si>
@@ -547,6 +547,27 @@
   </si>
   <si>
     <t>? CO homeostasis</t>
+  </si>
+  <si>
+    <t>Mech-Interference</t>
+  </si>
+  <si>
+    <t>hyper-CO interference</t>
+  </si>
+  <si>
+    <t>Crossover Interference: Shedding Light on the Evolution of Recombination</t>
+  </si>
+  <si>
+    <t>theo, simulations of interference variation</t>
+  </si>
+  <si>
+    <t>natural variation in COI</t>
+  </si>
+  <si>
+    <t>Wang Z, Shen B, Jiang J, Li J, Ma L. 2016. Effect of sex, age and genetics on crossover interference in cattle. Sci. Rep. 6:37698</t>
+  </si>
+  <si>
+    <t>Bauer E, Falque M,Walter H, Bauland C, Camisan C, et al. 2013. Intraspecific variation of recombination rate in maize. Genome Biol. 14:R103–1</t>
   </si>
 </sst>
 </file>
@@ -908,11 +929,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,8 +1180,45 @@
       <c r="A26">
         <v>2019</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2013</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2016</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1177,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added tabs for Discussion
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
-    <sheet name="DSB.DMC1" sheetId="7" r:id="rId2"/>
-    <sheet name="CO Rec landscale" sheetId="3" r:id="rId3"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId4"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId5"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId6"/>
-    <sheet name="SC general" sheetId="6" r:id="rId7"/>
+    <sheet name="Discussion1HetC" sheetId="8" r:id="rId2"/>
+    <sheet name="DSB.DMC1" sheetId="7" r:id="rId3"/>
+    <sheet name="CO Rec landscale" sheetId="3" r:id="rId4"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId5"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId6"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId7"/>
+    <sheet name="SC general" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -74,7 +75,7 @@
     <author>PETERSON, APRIL L</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +114,7 @@
     <author>PETERSON, APRIL L</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,10 +173,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Searching for references to bolter / support the prediction that female SC are longer than male
-*birds!
--Borodin papers
-*Fish</t>
+Searching for references to bolter / support the prediction that male and female IFD should be the same.
+- papers that cite Petkov 
+-citations within Payseur and Otto
+- citations within Shapley et al review
+- citations within WangR SC review
+- known oocyte cytology papers</t>
         </r>
       </text>
     </comment>
@@ -294,8 +297,45 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PETERSON, APRIL L</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PETERSON, APRIL L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Searching for references to bolter / support the prediction that female SC are longer than male
+*birds!
+-Borodin papers
+*Fish</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
   <si>
     <t>Year</t>
   </si>
@@ -569,12 +609,184 @@
   <si>
     <t>Bauer E, Falque M,Walter H, Bauland C, Camisan C, et al. 2013. Intraspecific variation of recombination rate in maize. Genome Biol. 14:R103–1</t>
   </si>
+  <si>
+    <t>SAC review</t>
+  </si>
+  <si>
+    <r>
+      <t>Lane, S., &amp; Kauppi, L. (2019). Meiotic spindle assembly checkpoint and aneuploidy in males versus females. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cellular and molecular life sciences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>76</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(6), 1135-1150. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**good review, good figures  SAC</t>
+    </r>
+  </si>
+  <si>
+    <t>Subramanian and hochwagen 2014 – great review on the meiotic checkpoint network (MCN) ATM and ATR main players signals</t>
+  </si>
+  <si>
+    <t>So et al 2019</t>
+  </si>
+  <si>
+    <t>Scahtten Sun 2009</t>
+  </si>
+  <si>
+    <t>Schuh Ellenburg 2007</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>A liquid-like spindle domain promotes acentrosomal spindle assembly in mammalian oocytes</t>
+  </si>
+  <si>
+    <t>acentrosome spindle</t>
+  </si>
+  <si>
+    <t>The Functional Significance of Centrosomes in MammalianMeiosis, Fertilization, Development, Nuclear Transfer, and Stem Cell Differentiation</t>
+  </si>
+  <si>
+    <t>main points to use</t>
+  </si>
+  <si>
+    <t>centrosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SpindleAssemblyin LiveMouseOocytesSelf-Organization of MTOCs Replaces CentrosomeFunctionduringAcentrosomal</t>
+  </si>
+  <si>
+    <t>MTOC in centrosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manadhar et al 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Ross and Normark 2015 </t>
+  </si>
+  <si>
+    <t>centrosome very conserved</t>
+  </si>
+  <si>
+    <t>Evolutionary problems in centrosome and centriole biology</t>
+  </si>
+  <si>
+    <t>NO such thing as centrosome inheretance</t>
+  </si>
+  <si>
+    <t>Centrosome Reduction During Gametogenesis and Its Significance1</t>
+  </si>
+  <si>
+    <t>centrosome reduction in sperm and oocyte</t>
+  </si>
+  <si>
+    <t>centrosome refs</t>
+  </si>
+  <si>
+    <t>Weird oocyte things</t>
+  </si>
+  <si>
+    <t>drive in oocytes</t>
+  </si>
+  <si>
+    <t>Ottolini</t>
+  </si>
+  <si>
+    <t>Genome-wide maps of recombination and chromosome segregation in human oocytes and embryos show selection for maternal recombination rates</t>
+  </si>
+  <si>
+    <t>Massive crossover elevation via combination of HEI10 and recq4a recq4b during Arabidopsis meiosis</t>
+  </si>
+  <si>
+    <t>Serra (Mercier Henderson)</t>
+  </si>
+  <si>
+    <t>(relationship between interference and more COs)</t>
+  </si>
+  <si>
+    <t>Spindle asymmetry drives non-Mendelian chromosome segregation</t>
+  </si>
+  <si>
+    <t>Akera (Lampson)</t>
+  </si>
+  <si>
+    <t>Molecular Strategies of Meiotic Cheating by Selfish Centromeres</t>
+  </si>
+  <si>
+    <t>mechismis of driving centr</t>
+  </si>
+  <si>
+    <t>Indirect Theory</t>
+  </si>
+  <si>
+    <t>Brandvain and Coop</t>
+  </si>
+  <si>
+    <t>Haig</t>
+  </si>
+  <si>
+    <t>Sardell and Kirkpatrick</t>
+  </si>
+  <si>
+    <t>Trivers</t>
+  </si>
+  <si>
+    <t>Lenormand Duthiel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +823,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -639,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -648,6 +883,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -929,11 +1167,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,25 +1437,42 @@
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="E30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>2013</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2016</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1233,6 +1488,233 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5">
+        <v>2019</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>2009</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>2007</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8">
+        <v>2015</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9">
+        <v>2005</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23">
+        <v>2017</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24">
+        <v>2019</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2019</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2012</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>2010</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1988</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2005</v>
+      </c>
+      <c r="C33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1342,7 +1824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1405,7 +1887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1502,7 +1984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1538,7 +2020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1574,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
seems to have somewhat fix bibtex references
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
     <sheet name="Discussion1HetC" sheetId="8" r:id="rId2"/>
-    <sheet name="DSB.DMC1" sheetId="7" r:id="rId3"/>
-    <sheet name="CO Rec landscale" sheetId="3" r:id="rId4"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId5"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId6"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId7"/>
-    <sheet name="SC general" sheetId="6" r:id="rId8"/>
+    <sheet name="Disc2maleEvo" sheetId="9" r:id="rId3"/>
+    <sheet name="DSB.DMC1" sheetId="7" r:id="rId4"/>
+    <sheet name="CO Rec landscale" sheetId="3" r:id="rId5"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId6"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId7"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId8"/>
+    <sheet name="SC general" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -335,7 +336,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="130">
   <si>
     <t>Year</t>
   </si>
@@ -780,6 +781,12 @@
   </si>
   <si>
     <t>Lenormand Duthiel</t>
+  </si>
+  <si>
+    <t>Raffoux?</t>
+  </si>
+  <si>
+    <t>Role of Cis, Trans, and Inbreeding Effects on Meiotic Recombination in Saccharomyces cerevisiae</t>
   </si>
 </sst>
 </file>
@@ -874,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -886,6 +893,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1167,11 +1175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1450,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="7">
         <v>2018</v>
       </c>
       <c r="B31" t="s">
@@ -1453,26 +1461,40 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>2013</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>2016</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1490,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1714,6 +1736,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1824,7 +1860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1887,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1984,7 +2020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2020,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2056,7 +2092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
transfered citations to the excel sheet
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
     <sheet name="Discussion1HetC" sheetId="8" r:id="rId2"/>
     <sheet name="Disc.Chromatin" sheetId="10" r:id="rId3"/>
     <sheet name="Disc.Typical.Landscape" sheetId="11" r:id="rId4"/>
-    <sheet name="Disc2maleEvo" sheetId="9" r:id="rId5"/>
-    <sheet name="DSB.DMC1" sheetId="7" r:id="rId6"/>
-    <sheet name="CO Rec landscale" sheetId="3" r:id="rId7"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId8"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId9"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId10"/>
-    <sheet name="SC general" sheetId="6" r:id="rId11"/>
+    <sheet name="COM.others" sheetId="12" r:id="rId5"/>
+    <sheet name="Disc2maleEvo" sheetId="9" r:id="rId6"/>
+    <sheet name="DSB.DMC1" sheetId="7" r:id="rId7"/>
+    <sheet name="CO Rec landscale" sheetId="3" r:id="rId8"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId9"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId10"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId11"/>
+    <sheet name="SC general" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -338,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
   <si>
     <t>Year</t>
   </si>
@@ -825,6 +826,30 @@
   </si>
   <si>
     <t>Cahoon Libuda</t>
+  </si>
+  <si>
+    <t>other COM, / nucleus membrane citations (Harper, Golubovskaya, &amp; Cande, 2004; Naranjo &amp; Corredor, 2008; Scherthan et al., 1996; Zickler &amp; Kleckner, 2016).</t>
+  </si>
+  <si>
+    <t>telomere guided movements  citations: (Bass et al.,</t>
+  </si>
+  <si>
+    <t>2000; Chacon, Delivani, &amp; Tolic, 2016; Curtis, Lukaszewski, &amp; Chrzastek, 1991; Ding, Yamamoto, Haraguchi, &amp; Hiraoka, 2004; Gerton &amp;</t>
+  </si>
+  <si>
+    <t>Hawley, 2005; Lee, Conrad, &amp; Dresser, 2012; Lefrancois, Rockmill,</t>
+  </si>
+  <si>
+    <t>Xie, Roeder, &amp; Snyder, 2016; Page &amp; Hawley, 2003)</t>
+  </si>
+  <si>
+    <t>Repair of DSB - CO</t>
+  </si>
+  <si>
+    <t>(Anderson &amp; Stack, 2005; Bass et al., 2000; Brown et al., 2005; Croft &amp; Jones, 1989; Higgins, Osman, Jones, &amp; Franklin, 2014; Klutstein &amp; Cooper, 2014, Lukaszewski, 1997; Pratto et al., 2014; Viera, Santos, &amp; Rufas, 2009;</t>
+  </si>
+  <si>
+    <t>Xiang, Miller, Ross, Alvarado, &amp; Hawley, 2014).</t>
   </si>
 </sst>
 </file>
@@ -1570,6 +1595,42 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1601,7 +1662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1941,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,6 +2013,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1965,7 +2081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -2076,7 +2192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -2139,7 +2255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2234,40 +2350,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
joting down ideas while editing
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="162">
   <si>
     <t>Year</t>
   </si>
@@ -851,12 +851,172 @@
   <si>
     <t>Xiang, Miller, Ross, Alvarado, &amp; Hawley, 2014).</t>
   </si>
+  <si>
+    <r>
+      <t>Dumont, J., &amp; Desai, A. (2012). Acentrosomal spindle assembly and chromosome segregation during oocyte meiosis. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Trends in cell biology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5), 241-249.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dumont 2012</t>
+  </si>
+  <si>
+    <t>acentrosom spindle and chrom segregation</t>
+  </si>
+  <si>
+    <r>
+      <t>Kyogoku, H., &amp; Kitajima, T. S. (2017). Large cytoplasm is linked to the error-prone nature of oocytes. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Developmental cell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3), 287-298.</t>
+    </r>
+  </si>
+  <si>
+    <t>Kyogoku</t>
+  </si>
+  <si>
+    <t>cytoplasm volume and SAC efficency</t>
+  </si>
+  <si>
+    <t>Rubin, Macaisne, and Huynh (2020)</t>
+  </si>
+  <si>
+    <t>rapid prophase movements</t>
+  </si>
+  <si>
+    <t>cohesion affected by crossover number and placement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">altendorf </t>
+  </si>
+  <si>
+    <r>
+      <t>van Veen, J. E., &amp; Hawley, R. S. (2003). Meiosis: when even two is a crowd. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Current Biology</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(21), R831-R833.</t>
+    </r>
+  </si>
+  <si>
+    <t>see cahoon libuda for more citations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -916,6 +1076,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -944,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -960,6 +1161,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1244,8 +1449,8 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,16 +1916,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1822,55 +2028,75 @@
         <v>108</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11">
+        <v>2012</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12">
+        <v>2017</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>112</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>2015</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>113</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23">
-        <v>2017</v>
-      </c>
-      <c r="C23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,57 +2104,71 @@
         <v>121</v>
       </c>
       <c r="B24">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C24" t="s">
         <v>119</v>
       </c>
       <c r="D24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25">
+        <v>2019</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>2019</v>
-      </c>
-      <c r="C29" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>1988</v>
+        <v>2010</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
+        <v>1988</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34">
         <v>2005</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2014,10 +2254,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A2:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,6 +2300,16 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2194,10 +2444,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,6 +2498,35 @@
       <c r="D7" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2003</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2019</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added to read papers
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="Disc2maleEvo" sheetId="9" r:id="rId6"/>
     <sheet name="DSB.DMC1" sheetId="7" r:id="rId7"/>
     <sheet name="CO Rec landscale" sheetId="3" r:id="rId8"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId9"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId10"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId11"/>
-    <sheet name="SC general" sheetId="6" r:id="rId12"/>
+    <sheet name="TOREAD" sheetId="13" r:id="rId9"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId10"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId11"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId12"/>
+    <sheet name="SC general" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -339,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="175">
   <si>
     <t>Year</t>
   </si>
@@ -1010,6 +1011,129 @@
   </si>
   <si>
     <t>see cahoon libuda for more citations</t>
+  </si>
+  <si>
+    <t>https://www.cell.com/current-biology/fulltext/S0960-9822(20)30423-1#.XpCNR-CfBHk.twitter</t>
+  </si>
+  <si>
+    <r>
+      <t>Samuk, Kieran, et al. "Natural selection shapes variation in genome-wide recombination rate in Drosophila pseudoobscura." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Current Biology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (2020).</t>
+    </r>
+  </si>
+  <si>
+    <t>Noor paper, adaptive variation Dmel</t>
+  </si>
+  <si>
+    <r>
+      <t>Aguilera, Paula, et al. "The nuclear pore complex prevents sister chromatid recombination during replicative senescence." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature Communications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 11.1 (2020): 1-13.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-019-13979-5</t>
+  </si>
+  <si>
+    <t>nuclear pore prevention of sister chromtid</t>
+  </si>
+  <si>
+    <r>
+      <t>Zhurinsky, Jacob, et al. "Effects of the microtubule nucleator Mto1 on chromosomal movement, DNA repair, and sister chromatid cohesion in fission yeast." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Molecular biology of the cell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 30.21 (2019): 2695-2708.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.molbiolcell.org/doi/full/10.1091/mbc.E19-05-0301</t>
+  </si>
+  <si>
+    <t>MT and chromatin cohesion in fission yeast</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s12275-019-8541-9</t>
+  </si>
+  <si>
+    <r>
+      <t>Hong, Soogil, et al. "The nature of meiotic chromosome dynamics and recombination in budding yeast." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Microbiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 57.4 (2019): 221-231.</t>
+    </r>
+  </si>
+  <si>
+    <t>chrm dynamics in budding yeast</t>
+  </si>
+  <si>
+    <t>TO READ PAPERS</t>
   </si>
 </sst>
 </file>
@@ -1797,6 +1921,103 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2015</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2016</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1831,7 +2052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1867,7 +2088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2446,7 +2667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -2535,98 +2756,72 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2015</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2016</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location=".XpCNR-CfBHk.twitter" display="https://www.cell.com/current-biology/fulltext/S0960-9822(20)30423-1 - .XpCNR-CfBHk.twitter"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more updates to figure scripts ect
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="255">
   <si>
     <t>Year</t>
   </si>
@@ -1846,12 +1846,137 @@
   <si>
     <t>National Center for Biotechnology Information, U.S. National Library of Medicine</t>
   </si>
+  <si>
+    <r>
+      <t>ElInati, E., Zielinska, A.P., McCarthy, A. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>et al.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> The BCL-2 pathway preserves mammalian genome integrity by eliminating recombination-defective oocytes. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nat Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>11, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2598 (2020). https://doi.org/10.1038/s41467-020-16441-z</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-020-16441-z#citeas</t>
+  </si>
+  <si>
+    <t>those zebra fish articles</t>
+  </si>
+  <si>
+    <r>
+      <t>Kochakpour, N., and P. B. Moens. "Sex-specific crossover patterns in Zebrafish (Danio rerio)." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Heredity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 100.5 (2008): 489-495.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/6801091/</t>
+  </si>
+  <si>
+    <r>
+      <t>Blokhina, Yana P., et al. "The telomere bouquet is a hub where meiotic double-strand breaks, synapsis, and stable homolog juxtaposition are coordinated in the zebrafish, Danio rerio." </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PLoS genetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 15.1 (2019).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosgenetics/article/file?type=printable&amp;id=10.1371/journal.pgen.1007854</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosgenetics/article/file?type=printable&amp;id=10.1371/journal.pgen.1007730</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1970,6 +2095,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2013,7 +2158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2066,6 +2211,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2698,524 +2844,535 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B116"/>
+  <dimension ref="B1:B117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="2:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B1" s="24" t="s">
+        <v>247</v>
+      </c>
+    </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+    <row r="30" spans="2:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+    <row r="31" spans="2:2" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+    <row r="32" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
+    <row r="33" spans="2:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+    <row r="34" spans="2:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+    <row r="35" spans="2:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
     </row>
-    <row r="37" spans="2:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="17"/>
+    </row>
+    <row r="38" spans="2:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="315" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="39" spans="2:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+    <row r="40" spans="2:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="17"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="17"/>
     </row>
-    <row r="47" spans="2:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="17"/>
+    </row>
+    <row r="48" spans="2:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="B48" s="13" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="17"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
     </row>
-    <row r="50" spans="2:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="17"/>
+    </row>
+    <row r="51" spans="2:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="17"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="17"/>
     </row>
-    <row r="53" spans="2:2" ht="315" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
+    </row>
+    <row r="54" spans="2:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="B54" s="13" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="13" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="17"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="17"/>
     </row>
-    <row r="59" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="13" t="s">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+    </row>
+    <row r="60" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="B60" s="13" t="s">
+    <row r="61" spans="2:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="B61" s="13" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="B61" s="13" t="s">
+    <row r="62" spans="2:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="B62" s="13" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="18" t="s">
+    <row r="63" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="17"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="17"/>
     </row>
-    <row r="65" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B65" s="13" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="17"/>
+    </row>
+    <row r="66" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="B66" s="13" t="s">
+    <row r="67" spans="2:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B67" s="13" t="s">
+    <row r="68" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="B68" s="13" t="s">
+    <row r="69" spans="2:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B69" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="B69" s="13" t="s">
+    <row r="70" spans="2:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="B70" s="13" t="s">
+    <row r="71" spans="2:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="B71" s="13" t="s">
+    <row r="72" spans="2:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="B72" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="B72" s="13" t="s">
+    <row r="73" spans="2:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="B73" s="13" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B73" s="13" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B74" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B75" s="13" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="17"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="17"/>
     </row>
-    <row r="77" spans="2:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="B77" s="13" t="s">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="17"/>
+    </row>
+    <row r="78" spans="2:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="B78" s="13" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="B78" s="13" t="s">
+    <row r="79" spans="2:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="B79" s="13" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="17"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="17"/>
     </row>
-    <row r="81" spans="2:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="B81" s="13" t="s">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="17"/>
+    </row>
+    <row r="82" spans="2:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="B82" s="13" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="B82" s="13" t="s">
+    <row r="83" spans="2:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="B83" s="13" t="s">
+    <row r="84" spans="2:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B84" s="13" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="B84" s="13" t="s">
+    <row r="85" spans="2:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="B85" s="13" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="17"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="17"/>
     </row>
-    <row r="87" spans="2:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="B87" s="13" t="s">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="17"/>
+    </row>
+    <row r="88" spans="2:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="B88" s="13" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="B88" s="13" t="s">
+    <row r="89" spans="2:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="B89" s="13" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="B89" s="13" t="s">
+    <row r="90" spans="2:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B90" s="13" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="91" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B91" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B92" s="13" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="B92" s="13" t="s">
+    <row r="93" spans="2:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="B93" s="13" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="B93" s="13" t="s">
+    <row r="94" spans="2:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="B94" s="13" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="B94" s="13" t="s">
+    <row r="95" spans="2:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="B95" s="13" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="17"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="17"/>
     </row>
-    <row r="97" spans="2:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="B97" s="13" t="s">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="17"/>
+    </row>
+    <row r="98" spans="2:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B98" s="13" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="17"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="17"/>
     </row>
-    <row r="100" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B100" s="13" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="17"/>
+    </row>
+    <row r="101" spans="2:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B101" s="13" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="B101" s="13" t="s">
+    <row r="102" spans="2:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="B102" s="13" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="B102" s="13" t="s">
+    <row r="103" spans="2:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="B103" s="13" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="17"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="17"/>
     </row>
-    <row r="105" spans="2:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="B105" s="13" t="s">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="17"/>
+    </row>
+    <row r="106" spans="2:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="B106" s="13" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="14"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="14"/>
     </row>
-    <row r="108" spans="2:2" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B108" s="19" t="s">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="14"/>
+    </row>
+    <row r="109" spans="2:2" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B109" s="19" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="20"/>
-    </row>
-    <row r="110" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B110" s="21" t="s">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="20"/>
+    </row>
+    <row r="111" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B111" s="21" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="22"/>
-    </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="23" t="s">
-        <v>242</v>
-      </c>
+      <c r="B112" s="22"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="B116" s="19" t="s">
+    <row r="117" spans="2:2" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="B117" s="19" t="s">
         <v>246</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
-    <hyperlink ref="B32" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/pubmed/11992253/"/>
-    <hyperlink ref="B33" r:id="rId3" display="https://www.ncbi.nlm.nih.gov/pubmed/17616720/"/>
-    <hyperlink ref="B34" r:id="rId4" display="https://www.ncbi.nlm.nih.gov/pubmed/9781043/"/>
-    <hyperlink ref="B37" r:id="rId5" display="https://www.ncbi.nlm.nih.gov/pubmed/9781043/"/>
-    <hyperlink ref="B38" r:id="rId6" display="https://www.ncbi.nlm.nih.gov/pubmed/12052900/"/>
-    <hyperlink ref="B39" r:id="rId7" display="https://www.ncbi.nlm.nih.gov/pubmed/14973780/"/>
-    <hyperlink ref="B40" r:id="rId8" display="https://www.ncbi.nlm.nih.gov/pubmed/10101178/"/>
-    <hyperlink ref="B41" r:id="rId9" display="https://www.ncbi.nlm.nih.gov/pubmed/12242241/"/>
-    <hyperlink ref="B42" r:id="rId10" display="https://www.ncbi.nlm.nih.gov/pubmed/18057311/"/>
-    <hyperlink ref="B43" r:id="rId11" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
-    <hyperlink ref="B44" r:id="rId12" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
-    <hyperlink ref="B47" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pubmed/6241455/"/>
-    <hyperlink ref="B50" r:id="rId14" display="https://www.ncbi.nlm.nih.gov/pubmed/8944012/"/>
-    <hyperlink ref="B53" r:id="rId15" display="https://www.ncbi.nlm.nih.gov/pubmed/12052900/"/>
-    <hyperlink ref="B54" r:id="rId16" display="https://www.ncbi.nlm.nih.gov/pubmed/10101178/"/>
-    <hyperlink ref="B55" r:id="rId17" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
-    <hyperlink ref="B56" r:id="rId18" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
-    <hyperlink ref="B59" r:id="rId19" display="https://www.ncbi.nlm.nih.gov/pubmed/8054979/"/>
-    <hyperlink ref="B60" r:id="rId20" display="https://www.ncbi.nlm.nih.gov/pubmed/9718341/"/>
-    <hyperlink ref="B61" r:id="rId21" display="https://www.ncbi.nlm.nih.gov/pubmed/12053178/"/>
-    <hyperlink ref="B62" r:id="rId22" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2735652/"/>
-    <hyperlink ref="B65" r:id="rId23" display="https://www.ncbi.nlm.nih.gov/pubmed/18057311/"/>
-    <hyperlink ref="B66" r:id="rId24" display="https://www.ncbi.nlm.nih.gov/pubmed/17298983/"/>
-    <hyperlink ref="B67" r:id="rId25" display="https://www.ncbi.nlm.nih.gov/pubmed/12750322/"/>
-    <hyperlink ref="B68" r:id="rId26" display="https://www.ncbi.nlm.nih.gov/pubmed/17696612/"/>
-    <hyperlink ref="B69" r:id="rId27" display="https://www.ncbi.nlm.nih.gov/pubmed/18787696/"/>
-    <hyperlink ref="B70" r:id="rId28" display="https://www.ncbi.nlm.nih.gov/pubmed/10385520/"/>
-    <hyperlink ref="B71" r:id="rId29" display="https://www.ncbi.nlm.nih.gov/pubmed/16307920/"/>
-    <hyperlink ref="B72" r:id="rId30" display="https://www.ncbi.nlm.nih.gov/pubmed/18430927/"/>
-    <hyperlink ref="B73" r:id="rId31" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
-    <hyperlink ref="B74" r:id="rId32" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
-    <hyperlink ref="B77" r:id="rId33" display="https://www.ncbi.nlm.nih.gov/pubmed/18502786/"/>
-    <hyperlink ref="B78" r:id="rId34" display="https://www.ncbi.nlm.nih.gov/pubmed/10801387/"/>
-    <hyperlink ref="B81" r:id="rId35" display="https://www.ncbi.nlm.nih.gov/pubmed/14973780/"/>
-    <hyperlink ref="B82" r:id="rId36" display="https://www.ncbi.nlm.nih.gov/pubmed/17989245/"/>
-    <hyperlink ref="B83" r:id="rId37" display="https://www.ncbi.nlm.nih.gov/pubmed/15485352/"/>
-    <hyperlink ref="B84" r:id="rId38" display="https://www.ncbi.nlm.nih.gov/pubmed/9718341/"/>
-    <hyperlink ref="B87" r:id="rId39" display="https://www.ncbi.nlm.nih.gov/pubmed/9499419/"/>
-    <hyperlink ref="B88" r:id="rId40" display="https://www.ncbi.nlm.nih.gov/pubmed/18369452/"/>
-    <hyperlink ref="B89" r:id="rId41" display="https://www.ncbi.nlm.nih.gov/pubmed/1997383/"/>
-    <hyperlink ref="B90" r:id="rId42" display="https://www.ncbi.nlm.nih.gov/pubmed/12151449/"/>
-    <hyperlink ref="B91" r:id="rId43" display="https://www.ncbi.nlm.nih.gov/pubmed/10942110/"/>
-    <hyperlink ref="B92" r:id="rId44" display="https://www.ncbi.nlm.nih.gov/pubmed/12137856/"/>
-    <hyperlink ref="B93" r:id="rId45" display="https://www.ncbi.nlm.nih.gov/pubmed/6241455/"/>
-    <hyperlink ref="B94" r:id="rId46" display="https://www.ncbi.nlm.nih.gov/pubmed/8236460/"/>
-    <hyperlink ref="B97" r:id="rId47" display="https://www.ncbi.nlm.nih.gov/pubmed/11283700/"/>
-    <hyperlink ref="B100" r:id="rId48" display="https://www.ncbi.nlm.nih.gov/pubmed/9285774/"/>
-    <hyperlink ref="B101" r:id="rId49" display="https://www.ncbi.nlm.nih.gov/pubmed/18369452/"/>
-    <hyperlink ref="B102" r:id="rId50" display="https://www.ncbi.nlm.nih.gov/pubmed/17584770/"/>
-    <hyperlink ref="B105" r:id="rId51" display="https://www.ncbi.nlm.nih.gov/pubmed/9088645/"/>
-    <hyperlink ref="B110" r:id="rId52" display="https://www.nlm.nih.gov/privacy.html"/>
-    <hyperlink ref="B112" r:id="rId53" tooltip="NLM" display="https://www.nlm.nih.gov/"/>
-    <hyperlink ref="B113" r:id="rId54" tooltip="NIH" display="https://www.nih.gov/"/>
-    <hyperlink ref="B114" r:id="rId55" tooltip="DHHS" display="https://www.hhs.gov/"/>
-    <hyperlink ref="B115" r:id="rId56" tooltip="USA.gov" display="https://www.usa.gov/"/>
+    <hyperlink ref="B30" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
+    <hyperlink ref="B33" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/pubmed/11992253/"/>
+    <hyperlink ref="B34" r:id="rId3" display="https://www.ncbi.nlm.nih.gov/pubmed/17616720/"/>
+    <hyperlink ref="B35" r:id="rId4" display="https://www.ncbi.nlm.nih.gov/pubmed/9781043/"/>
+    <hyperlink ref="B38" r:id="rId5" display="https://www.ncbi.nlm.nih.gov/pubmed/9781043/"/>
+    <hyperlink ref="B39" r:id="rId6" display="https://www.ncbi.nlm.nih.gov/pubmed/12052900/"/>
+    <hyperlink ref="B40" r:id="rId7" display="https://www.ncbi.nlm.nih.gov/pubmed/14973780/"/>
+    <hyperlink ref="B41" r:id="rId8" display="https://www.ncbi.nlm.nih.gov/pubmed/10101178/"/>
+    <hyperlink ref="B42" r:id="rId9" display="https://www.ncbi.nlm.nih.gov/pubmed/12242241/"/>
+    <hyperlink ref="B43" r:id="rId10" display="https://www.ncbi.nlm.nih.gov/pubmed/18057311/"/>
+    <hyperlink ref="B44" r:id="rId11" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
+    <hyperlink ref="B45" r:id="rId12" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
+    <hyperlink ref="B48" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pubmed/6241455/"/>
+    <hyperlink ref="B51" r:id="rId14" display="https://www.ncbi.nlm.nih.gov/pubmed/8944012/"/>
+    <hyperlink ref="B54" r:id="rId15" display="https://www.ncbi.nlm.nih.gov/pubmed/12052900/"/>
+    <hyperlink ref="B55" r:id="rId16" display="https://www.ncbi.nlm.nih.gov/pubmed/10101178/"/>
+    <hyperlink ref="B56" r:id="rId17" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
+    <hyperlink ref="B57" r:id="rId18" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
+    <hyperlink ref="B60" r:id="rId19" display="https://www.ncbi.nlm.nih.gov/pubmed/8054979/"/>
+    <hyperlink ref="B61" r:id="rId20" display="https://www.ncbi.nlm.nih.gov/pubmed/9718341/"/>
+    <hyperlink ref="B62" r:id="rId21" display="https://www.ncbi.nlm.nih.gov/pubmed/12053178/"/>
+    <hyperlink ref="B63" r:id="rId22" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2735652/"/>
+    <hyperlink ref="B66" r:id="rId23" display="https://www.ncbi.nlm.nih.gov/pubmed/18057311/"/>
+    <hyperlink ref="B67" r:id="rId24" display="https://www.ncbi.nlm.nih.gov/pubmed/17298983/"/>
+    <hyperlink ref="B68" r:id="rId25" display="https://www.ncbi.nlm.nih.gov/pubmed/12750322/"/>
+    <hyperlink ref="B69" r:id="rId26" display="https://www.ncbi.nlm.nih.gov/pubmed/17696612/"/>
+    <hyperlink ref="B70" r:id="rId27" display="https://www.ncbi.nlm.nih.gov/pubmed/18787696/"/>
+    <hyperlink ref="B71" r:id="rId28" display="https://www.ncbi.nlm.nih.gov/pubmed/10385520/"/>
+    <hyperlink ref="B72" r:id="rId29" display="https://www.ncbi.nlm.nih.gov/pubmed/16307920/"/>
+    <hyperlink ref="B73" r:id="rId30" display="https://www.ncbi.nlm.nih.gov/pubmed/18430927/"/>
+    <hyperlink ref="B74" r:id="rId31" display="https://www.ncbi.nlm.nih.gov/pubmed/15558497/"/>
+    <hyperlink ref="B75" r:id="rId32" display="https://www.ncbi.nlm.nih.gov/pubmed/16820117/"/>
+    <hyperlink ref="B78" r:id="rId33" display="https://www.ncbi.nlm.nih.gov/pubmed/18502786/"/>
+    <hyperlink ref="B79" r:id="rId34" display="https://www.ncbi.nlm.nih.gov/pubmed/10801387/"/>
+    <hyperlink ref="B82" r:id="rId35" display="https://www.ncbi.nlm.nih.gov/pubmed/14973780/"/>
+    <hyperlink ref="B83" r:id="rId36" display="https://www.ncbi.nlm.nih.gov/pubmed/17989245/"/>
+    <hyperlink ref="B84" r:id="rId37" display="https://www.ncbi.nlm.nih.gov/pubmed/15485352/"/>
+    <hyperlink ref="B85" r:id="rId38" display="https://www.ncbi.nlm.nih.gov/pubmed/9718341/"/>
+    <hyperlink ref="B88" r:id="rId39" display="https://www.ncbi.nlm.nih.gov/pubmed/9499419/"/>
+    <hyperlink ref="B89" r:id="rId40" display="https://www.ncbi.nlm.nih.gov/pubmed/18369452/"/>
+    <hyperlink ref="B90" r:id="rId41" display="https://www.ncbi.nlm.nih.gov/pubmed/1997383/"/>
+    <hyperlink ref="B91" r:id="rId42" display="https://www.ncbi.nlm.nih.gov/pubmed/12151449/"/>
+    <hyperlink ref="B92" r:id="rId43" display="https://www.ncbi.nlm.nih.gov/pubmed/10942110/"/>
+    <hyperlink ref="B93" r:id="rId44" display="https://www.ncbi.nlm.nih.gov/pubmed/12137856/"/>
+    <hyperlink ref="B94" r:id="rId45" display="https://www.ncbi.nlm.nih.gov/pubmed/6241455/"/>
+    <hyperlink ref="B95" r:id="rId46" display="https://www.ncbi.nlm.nih.gov/pubmed/8236460/"/>
+    <hyperlink ref="B98" r:id="rId47" display="https://www.ncbi.nlm.nih.gov/pubmed/11283700/"/>
+    <hyperlink ref="B101" r:id="rId48" display="https://www.ncbi.nlm.nih.gov/pubmed/9285774/"/>
+    <hyperlink ref="B102" r:id="rId49" display="https://www.ncbi.nlm.nih.gov/pubmed/18369452/"/>
+    <hyperlink ref="B103" r:id="rId50" display="https://www.ncbi.nlm.nih.gov/pubmed/17584770/"/>
+    <hyperlink ref="B106" r:id="rId51" display="https://www.ncbi.nlm.nih.gov/pubmed/9088645/"/>
+    <hyperlink ref="B111" r:id="rId52" display="https://www.nlm.nih.gov/privacy.html"/>
+    <hyperlink ref="B113" r:id="rId53" tooltip="NLM" display="https://www.nlm.nih.gov/"/>
+    <hyperlink ref="B114" r:id="rId54" tooltip="NIH" display="https://www.nih.gov/"/>
+    <hyperlink ref="B115" r:id="rId55" tooltip="DHHS" display="https://www.hhs.gov/"/>
+    <hyperlink ref="B116" r:id="rId56" tooltip="USA.gov" display="https://www.usa.gov/"/>
+    <hyperlink ref="B2" r:id="rId57" location="citeas" display="https://www.nature.com/articles/s41467-020-16441-z - citeas"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 
@@ -4143,10 +4300,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,14 +4360,43 @@
         <v>173</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location=".XpCNR-CfBHk.twitter" display="https://www.cell.com/current-biology/fulltext/S0960-9822(20)30423-1 - .XpCNR-CfBHk.twitter"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A9" r:id="rId5"/>
+    <hyperlink ref="A11" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates from final v2 files
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -343,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="263">
   <si>
     <t>Year</t>
   </si>
@@ -1970,6 +1970,30 @@
   </si>
   <si>
     <t>https://journals.plos.org/plosgenetics/article/file?type=printable&amp;id=10.1371/journal.pgen.1007730</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/15384101.2017.1319689</t>
+  </si>
+  <si>
+    <t>Crossover maturation inefficiency and aneuploidy in human female meiosis</t>
+  </si>
+  <si>
+    <t>Crossover Position Drives Chromosome Remodeling for Accurate Meiotic Chromosome Segregation</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0960982220301597?casa_token=4xwgMK4DnJwAAAAA:LkbzlHftRN4u2nTzCgMkfGmKJYpoBE4o4_GDo5d7Ch0eHCqRlY9f4sxYex6BCPf7n1OboqB1zYs</t>
+  </si>
+  <si>
+    <t>Role of cleavage by separase of the Rec8 kleisin subunit of cohesin during mammalian meiosis I</t>
+  </si>
+  <si>
+    <t>https://jcs.biologists.org/content/122/15/2686.short</t>
+  </si>
+  <si>
+    <t>The Regulation and Function of Cohesin and Condensin in Mammalian Oocytes and Spermatocytes</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-319-60855-6_15</t>
   </si>
 </sst>
 </file>
@@ -4300,10 +4324,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,6 +4410,38 @@
         <v>253</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B18" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location=".XpCNR-CfBHk.twitter" display="https://www.cell.com/current-biology/fulltext/S0960-9822(20)30423-1 - .XpCNR-CfBHk.twitter"/>
@@ -4395,8 +4451,12 @@
     <hyperlink ref="A9" r:id="rId5"/>
     <hyperlink ref="A11" r:id="rId6"/>
     <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A15" r:id="rId8"/>
+    <hyperlink ref="A17" r:id="rId9"/>
+    <hyperlink ref="A14" r:id="rId10"/>
+    <hyperlink ref="A18" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
notes and links for refs regarding synchornized chrm in sperm
</commit_message>
<xml_diff>
--- a/Ref_organization.xlsx
+++ b/Ref_organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="12195" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Interference sources" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="DSB.DMC1" sheetId="7" r:id="rId7"/>
     <sheet name="CO Rec landscale" sheetId="3" r:id="rId8"/>
     <sheet name="TOREAD" sheetId="13" r:id="rId9"/>
-    <sheet name="oocytes" sheetId="14" r:id="rId10"/>
-    <sheet name="popgen theories, dynamics" sheetId="15" r:id="rId11"/>
-    <sheet name="House mouse pop gen" sheetId="16" r:id="rId12"/>
-    <sheet name="sex specific SC length" sheetId="2" r:id="rId13"/>
-    <sheet name="main kleckner papers" sheetId="5" r:id="rId14"/>
-    <sheet name="within species difs, rec" sheetId="4" r:id="rId15"/>
-    <sheet name="SC general" sheetId="6" r:id="rId16"/>
+    <sheet name="synchornization of chrm" sheetId="17" r:id="rId10"/>
+    <sheet name="oocytes" sheetId="14" r:id="rId11"/>
+    <sheet name="popgen theories, dynamics" sheetId="15" r:id="rId12"/>
+    <sheet name="House mouse pop gen" sheetId="16" r:id="rId13"/>
+    <sheet name="sex specific SC length" sheetId="2" r:id="rId14"/>
+    <sheet name="main kleckner papers" sheetId="5" r:id="rId15"/>
+    <sheet name="within species difs, rec" sheetId="4" r:id="rId16"/>
+    <sheet name="SC general" sheetId="6" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -343,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="293">
   <si>
     <t>Year</t>
   </si>
@@ -2007,12 +2008,90 @@
   <si>
     <t>https://www.nature.com/articles/s41586-020-2347-0</t>
   </si>
+  <si>
+    <t>https://www.g3journal.org/content/10/5/1765.long</t>
+  </si>
+  <si>
+    <t>Phosphorylated proteins are involved in sister-chromatid arm cohesion during meiosis I</t>
+  </si>
+  <si>
+    <t>https://jcs.biologists.org/content/joces/112/17/2957.full.pdf</t>
+  </si>
+  <si>
+    <t>Temporally and spatially selective loss of Rec8 protein from meiotic chromosomes during mammalian meiosis</t>
+  </si>
+  <si>
+    <t>https://jcs.biologists.org/content/joces/116/13/2781.full.pdf</t>
+  </si>
+  <si>
+    <t>Chromatid Cores in Meiotic Chromosome Structure and Segregation</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/7050_2006_023</t>
+  </si>
+  <si>
+    <t>Chromosome Choreography: The Meiotic Ballet</t>
+  </si>
+  <si>
+    <t>https://science.sciencemag.org/content/301/5634/785?casa_token=kGD4w9TbscMAAAAA:O7rBeYP-bE1AZ3LDbqgUv7aenGrXBWn4_ycq68XFkQoCbSsEE82a1IgF0j73txq8Ekx7x-agc6xiqL8</t>
+  </si>
+  <si>
+    <t>Sister chromatid cohesion and recombination in meiosis</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/content/pdf/10.1007/s004120050408.pdf</t>
+  </si>
+  <si>
+    <t>Kudo</t>
+  </si>
+  <si>
+    <t>Chapter One - Cohesin in Gametogenesis</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/B9780124160248000015?casa_token=8uCEIeXCqd4AAAAA:T_wQWClf3rGwPFL9aw_JpHkxIJTBbQVvq6wq3W1rRXO0ynoQLBElp8tJbvZi9Wq5IBUBllJYDUM</t>
+  </si>
+  <si>
+    <t>McNicoll</t>
+  </si>
+  <si>
+    <t>Meiotic spindle assembly checkpoint and aneuploidy in males versus females</t>
+  </si>
+  <si>
+    <t>Lane Kauppi</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00018-018-2986-6</t>
+  </si>
+  <si>
+    <t>Advances and Surprises in a Decade of Oocyte Meiosis Research</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/32538429/</t>
+  </si>
+  <si>
+    <t>Meiotic Recombination: The Essence of Heredity</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>https://cshperspectives.cshlp.org/content/7/12/a016618.full</t>
+  </si>
+  <si>
+    <t>The spindle checkpoint and chromosome segregation in meiosis</t>
+  </si>
+  <si>
+    <t>Gorbsky</t>
+  </si>
+  <si>
+    <t>https://febs.onlinelibrary.wiley.com/doi/epdf/10.1111/febs.13166</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2151,6 +2230,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2194,7 +2279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2248,6 +2333,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2880,6 +2966,143 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A14" r:id="rId4"/>
+    <hyperlink ref="A13" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId6"/>
+    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A11" r:id="rId8"/>
+    <hyperlink ref="A17" r:id="rId9"/>
+    <hyperlink ref="A18" r:id="rId10"/>
+    <hyperlink ref="A1" r:id="rId11"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3412,7 +3635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
@@ -3438,7 +3661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
@@ -3498,7 +3721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -3595,7 +3818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -3631,7 +3854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -3667,7 +3890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4336,10 +4559,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4396,77 +4619,94 @@
         <v>173</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B13" t="s">
-        <v>265</v>
+        <v>251</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B14" t="s">
-        <v>259</v>
+        <v>254</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B17" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4476,17 +4716,18 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A9" r:id="rId5"/>
-    <hyperlink ref="A11" r:id="rId6"/>
-    <hyperlink ref="A10" r:id="rId7"/>
-    <hyperlink ref="A15" r:id="rId8"/>
-    <hyperlink ref="A17" r:id="rId9"/>
-    <hyperlink ref="A14" r:id="rId10"/>
-    <hyperlink ref="A18" r:id="rId11"/>
-    <hyperlink ref="A21" r:id="rId12"/>
-    <hyperlink ref="A13" r:id="rId13"/>
+    <hyperlink ref="A13" r:id="rId5"/>
+    <hyperlink ref="A15" r:id="rId6"/>
+    <hyperlink ref="A14" r:id="rId7"/>
+    <hyperlink ref="A19" r:id="rId8"/>
+    <hyperlink ref="A21" r:id="rId9"/>
+    <hyperlink ref="A18" r:id="rId10"/>
+    <hyperlink ref="A22" r:id="rId11"/>
+    <hyperlink ref="A25" r:id="rId12"/>
+    <hyperlink ref="A17" r:id="rId13"/>
+    <hyperlink ref="A6" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>